<commit_message>
Agregadas algunas clases de equivalencia de los casos de prueba TP12
</commit_message>
<xml_diff>
--- a/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
+++ b/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documentos\2019-UTN-FRC-ISW-4K2-G7-TP5\Trabajos\Trabajos Prácticos\Prácticos Evaluables\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2B470A-87DE-4DC4-AF31-C5E6EECDCD38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89259D0A-327C-456D-AFC5-894BE1090D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="127">
   <si>
     <t>TC_001</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Detalle pedido</t>
-  </si>
-  <si>
     <t>Realización de pedido exitosa de "lo que sea" en efectivo, "lo antes posible".</t>
   </si>
   <si>
@@ -405,6 +402,21 @@
   </si>
   <si>
     <t>1- El solicitante selecciona la opción "Lo que sea". 2- El solicitante ingresa el detalle del pedido = "Auriculares Sony MDR-E9LP Negro". 3- El solicitante ingresa del comercio la calle = "Obispo Trejo". 4- El solicitante ingresa del comercio número = "410". 5- El solicitante selecciona del comercio la ciudad = "Córdoba". 6- El solicitante ingresa del domicilio de entrega la calle = "Tucumán". 7- El solicitante ingresa del domicilio de entrega el número = "172". 8- El solicitante selecciona del domicilio de entrega la ciudad = "Córdoba". 9- El solicitante selecciona la forma de pago = "Tarjeta VISA". 10- El solicitante ingresa el número de la tarjeta 5105105105105100. 11- El solicitante ingresa el nombre y apellido del titular. 12- El solicitante ingresa fecha de vencimiento de la tarjeta 09/20. 13- El solicitante ingresa CVC 087. 14- El solicitante selecciona tiempo de entrega = "Lo antes posible". 15- El solicitante selecciona la opción "Realizar pedido".</t>
+  </si>
+  <si>
+    <t>1-Numero de tarjeta valido.2-CVC de la tarjeta valido.3-Numero de tarjeta que comienza con 4.4-Numero de caracteres de la tarjeta=13.5-Fecha de vencimiento de tarjeta &gt; fecha actual.6-Detalle de pedido</t>
+  </si>
+  <si>
+    <t>1-Monto &gt; 0.2-Fecha y hora de entrega &gt; fecha y hora actual.3-Detalle de pedido valido</t>
+  </si>
+  <si>
+    <t>1-Detalle de  pedido valido.2-Monto &gt; 0.</t>
+  </si>
+  <si>
+    <t>1-Monto &gt; 0.2-Tamaño de imagen &lt; 5Mb.3-Detalle de pedio valido</t>
+  </si>
+  <si>
+    <t>1-Monto &gt; 0.2-Detalle de pedio valido</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1718,8 @@
   <dimension ref="A1:AS73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="131" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2065,19 +2077,19 @@
         <v>86</v>
       </c>
       <c r="C11" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>88</v>
-      </c>
       <c r="E11" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="15"/>
@@ -2108,18 +2120,20 @@
       <c r="B12" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="D12" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="15"/>
@@ -2148,20 +2162,22 @@
         <v>41</v>
       </c>
       <c r="B13" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21" t="s">
-        <v>92</v>
-      </c>
       <c r="E13" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="15"/>
@@ -2190,20 +2206,22 @@
         <v>42</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="21"/>
+        <v>98</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>125</v>
+      </c>
       <c r="D14" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="15"/>
@@ -2232,20 +2250,22 @@
         <v>43</v>
       </c>
       <c r="B15" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21" t="s">
-        <v>100</v>
-      </c>
       <c r="E15" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="15"/>
@@ -2274,20 +2294,20 @@
         <v>44</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="26" t="s">
+      <c r="G16" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>108</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="15"/>
@@ -2316,20 +2336,20 @@
         <v>45</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="26" t="s">
+      <c r="G17" s="26" t="s">
         <v>110</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="15"/>
@@ -2358,20 +2378,20 @@
         <v>46</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F18" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="26" t="s">
         <v>112</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>113</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="15"/>
@@ -2400,20 +2420,20 @@
         <v>47</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="26" t="s">
+      <c r="G19" s="26" t="s">
         <v>116</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>117</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="15"/>
@@ -2442,20 +2462,20 @@
         <v>48</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="26" t="s">
+      <c r="G20" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>120</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="15"/>
@@ -2484,20 +2504,20 @@
         <v>49</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>122</v>
-      </c>
       <c r="G21" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="15"/>
@@ -4640,6 +4660,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4765,24 +4802,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4798,22 +4836,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agregadas nuevas clases de equivalencia de casos de prueba TP12
</commit_message>
<xml_diff>
--- a/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
+++ b/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documentos\2019-UTN-FRC-ISW-4K2-G7-TP5\Trabajos\Trabajos Prácticos\Prácticos Evaluables\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89259D0A-327C-456D-AFC5-894BE1090D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8B40AA-8EA1-405C-8EEC-F9895229A8DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>TC_001</t>
   </si>
@@ -404,9 +404,6 @@
     <t>1- El solicitante selecciona la opción "Lo que sea". 2- El solicitante ingresa el detalle del pedido = "Auriculares Sony MDR-E9LP Negro". 3- El solicitante ingresa del comercio la calle = "Obispo Trejo". 4- El solicitante ingresa del comercio número = "410". 5- El solicitante selecciona del comercio la ciudad = "Córdoba". 6- El solicitante ingresa del domicilio de entrega la calle = "Tucumán". 7- El solicitante ingresa del domicilio de entrega el número = "172". 8- El solicitante selecciona del domicilio de entrega la ciudad = "Córdoba". 9- El solicitante selecciona la forma de pago = "Tarjeta VISA". 10- El solicitante ingresa el número de la tarjeta 5105105105105100. 11- El solicitante ingresa el nombre y apellido del titular. 12- El solicitante ingresa fecha de vencimiento de la tarjeta 09/20. 13- El solicitante ingresa CVC 087. 14- El solicitante selecciona tiempo de entrega = "Lo antes posible". 15- El solicitante selecciona la opción "Realizar pedido".</t>
   </si>
   <si>
-    <t>1-Numero de tarjeta valido.2-CVC de la tarjeta valido.3-Numero de tarjeta que comienza con 4.4-Numero de caracteres de la tarjeta=13.5-Fecha de vencimiento de tarjeta &gt; fecha actual.6-Detalle de pedido</t>
-  </si>
-  <si>
     <t>1-Monto &gt; 0.2-Fecha y hora de entrega &gt; fecha y hora actual.3-Detalle de pedido valido</t>
   </si>
   <si>
@@ -417,6 +414,24 @@
   </si>
   <si>
     <t>1-Monto &gt; 0.2-Detalle de pedio valido</t>
+  </si>
+  <si>
+    <t>1-Detalle de pedio no valido</t>
+  </si>
+  <si>
+    <t>1-Monto no valido.2-Detalle de pedio valido</t>
+  </si>
+  <si>
+    <t>1-Fecha y hora de entrega &lt; Fecha y hora actual.</t>
+  </si>
+  <si>
+    <t>1-primeros numeros de la tarjeta &gt;=51.2Primeros numeros de la tarjeta &lt;=55.</t>
+  </si>
+  <si>
+    <t>1-Detalle de pedido valido.2-Monto &gt; 0.3-Numero de tarjeta no valido. 4-CVC de la tarjeta no valido.5-Numero de tarjeta no comienza con 4.6-Digitos de la tarjeta &gt; 13.7-Digitos de la tarjeta &lt; 13.8-Longitud de CVC &lt;3.9-Fecha de vencimiento de tarjeta &lt; Fecha actual</t>
+  </si>
+  <si>
+    <t>1-Numero de tarjeta valido.2-CVC de la tarjeta valido.3-Primer numero de tarjeta = 4.4-Digitos de la tarjeta=13.5-Fecha de vencimiento de tarjeta &gt; fecha actual.6-Detalle de pedido valido.7-Longitud de CVC = 3.</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1733,8 @@
   <dimension ref="A1:AS73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="131" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2077,7 +2092,7 @@
         <v>86</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>87</v>
@@ -2121,7 +2136,7 @@
         <v>86</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>89</v>
@@ -2165,7 +2180,7 @@
         <v>90</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>91</v>
@@ -2209,7 +2224,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>93</v>
@@ -2253,7 +2268,7 @@
         <v>98</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>99</v>
@@ -2296,7 +2311,9 @@
       <c r="B16" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="21" t="s">
+        <v>126</v>
+      </c>
       <c r="D16" s="21" t="s">
         <v>105</v>
       </c>
@@ -2380,7 +2397,9 @@
       <c r="B18" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="D18" s="21" t="s">
         <v>113</v>
       </c>
@@ -2422,7 +2441,9 @@
       <c r="B19" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>128</v>
+      </c>
       <c r="D19" s="21" t="s">
         <v>114</v>
       </c>
@@ -2457,14 +2478,16 @@
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
     </row>
-    <row r="20" spans="1:45" ht="264" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" ht="324" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="21" t="s">
+        <v>130</v>
+      </c>
       <c r="D20" s="21" t="s">
         <v>117</v>
       </c>
@@ -2506,7 +2529,9 @@
       <c r="B21" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="21" t="s">
+        <v>129</v>
+      </c>
       <c r="D21" s="21" t="s">
         <v>120</v>
       </c>
@@ -4660,23 +4685,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4802,10 +4810,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4821,19 +4856,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agregadas mas clases de equivalencia para casos de prueba TP12
</commit_message>
<xml_diff>
--- a/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
+++ b/Trabajos/Trabajos Prácticos/Prácticos Evaluables/TP12/Casos_De_Prueba_TP12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documentos\2019-UTN-FRC-ISW-4K2-G7-TP5\Trabajos\Trabajos Prácticos\Prácticos Evaluables\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8B40AA-8EA1-405C-8EEC-F9895229A8DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A7A1E1-5535-470E-B122-D985B2E9A93D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
   <si>
     <t>TC_001</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>1-Numero de tarjeta valido.2-CVC de la tarjeta valido.3-Primer numero de tarjeta = 4.4-Digitos de la tarjeta=13.5-Fecha de vencimiento de tarjeta &gt; fecha actual.6-Detalle de pedido valido.7-Longitud de CVC = 3.</t>
+  </si>
+  <si>
+    <t>1-Direccion de comercio no valido</t>
   </si>
 </sst>
 </file>
@@ -1733,8 +1736,8 @@
   <dimension ref="A1:AS73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="131" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2355,7 +2358,9 @@
       <c r="B17" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="D17" s="21" t="s">
         <v>108</v>
       </c>
@@ -4685,6 +4690,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -4810,24 +4832,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4843,22 +4866,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>